<commit_message>
Fix psychologyGrad image name
</commit_message>
<xml_diff>
--- a/collegeGrads/catalog_products.xlsx
+++ b/collegeGrads/catalog_products.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="242">
   <si>
     <t># Required | A unique content ID for the item. Use the item's SKU if you can. Each content ID must appear only once in your catalog. To run dynamic ads this ID must exactly match the content ID for the same item in your Meta Pixel code. Character limit: 100</t>
   </si>
@@ -291,13 +291,25 @@
     <t>Software &gt; Digital Goods &amp; Currency &gt; Document Templates</t>
   </si>
   <si>
-    <t>221,electronics &gt; software</t>
+    <t>electronics &gt; software</t>
   </si>
   <si>
     <t>19 USD</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:00</t>
+  </si>
+  <si>
+    <t>neon</t>
+  </si>
+  <si>
+    <t>one-size</t>
+  </si>
+  <si>
     <t>digital</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
   <si>
     <t>US:0.0 USD</t>
@@ -338,6 +350,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/anthroplogyGrad.png</t>
   </si>
   <si>
+    <t>221,electronics &gt; software</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/anthropologyGrad.mov</t>
   </si>
   <si>
@@ -358,6 +376,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/artGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:01</t>
+  </si>
+  <si>
+    <t>red and orange</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/artGrad.mov</t>
   </si>
   <si>
@@ -377,6 +401,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/biologyGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:02</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/biologyGrad.mov</t>
   </si>
   <si>
@@ -395,6 +425,9 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/biologyGrad_B.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:03</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/biologyGrad_B.mov</t>
   </si>
   <si>
@@ -407,13 +440,22 @@
     <t>blank</t>
   </si>
   <si>
-    <t>0 USD</t>
+    <t>57 USD</t>
   </si>
   <si>
     <t>https://irenes-ventures.shop/portfolio-website-blank</t>
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/blank.png</t>
+  </si>
+  <si>
+    <t>25 USD</t>
+  </si>
+  <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:04</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
   <si>
     <t>7</t>
@@ -432,6 +474,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/chemistryGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:05</t>
+  </si>
+  <si>
+    <t>pastels</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/chemistryGrad.mov</t>
   </si>
   <si>
@@ -450,9 +498,15 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/civil-engineeringGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:06</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/civil-engineeringGrad.mov</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>Early Childhood Education</t>
   </si>
   <si>
@@ -465,10 +519,16 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/early-childhood-educationGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:07</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/early-childhood-educationGrad.mov</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>Electrical Engineering</t>
@@ -483,10 +543,16 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/electrical-engineeringGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:08</t>
+  </si>
+  <si>
+    <t>deep navy blue</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/electrical-engineeringGrad.mov</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>Electrical Engineering B</t>
@@ -501,10 +567,13 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/electrical-engineeringGrad_B.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:09</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/electrical-engineeringGrad_B.mov</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>Finance</t>
@@ -517,6 +586,12 @@
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/financeGrad.png</t>
+  </si>
+  <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:10</t>
+  </si>
+  <si>
+    <t>ruby red and cream</t>
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/financeGrad.mov</t>
@@ -542,6 +617,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/historyGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:11</t>
+  </si>
+  <si>
+    <t>beige</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/historyGrad.mov</t>
   </si>
   <si>
@@ -560,6 +641,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/linguisticsGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:12</t>
+  </si>
+  <si>
+    <t>multicolored</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/linguisticsGrad.mov</t>
   </si>
   <si>
@@ -576,6 +663,12 @@
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/physicsGrad.png</t>
+  </si>
+  <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:13</t>
+  </si>
+  <si>
+    <t>purple</t>
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/physicsGrad.mov</t>
@@ -598,6 +691,9 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/psychologyGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:14</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/psychologyGrad.mov</t>
   </si>
   <si>
@@ -617,6 +713,12 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/spanishGrad.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:15</t>
+  </si>
+  <si>
+    <t>yellow to blue gradient</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/spanishGrad.mov</t>
   </si>
   <si>
@@ -635,6 +737,9 @@
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/spanishGrad_B.png</t>
   </si>
   <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:16</t>
+  </si>
+  <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/spanishGrad_B.mov</t>
   </si>
   <si>
@@ -651,6 +756,12 @@
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/images/statisticsGrad.png</t>
+  </si>
+  <si>
+    <t>2025-12-27T00:00-07:00/2026-01-31T23:59-07:17</t>
+  </si>
+  <si>
+    <t>rainbow cloud</t>
   </si>
   <si>
     <t>https://irenelangkilde.github.io/Webworks/collegeGrads/assets/videos/statisticsGrad.mov</t>
@@ -1333,44 +1444,62 @@
       <c r="M4" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N4" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O4" s="5">
         <v>1.0</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="Q4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S4" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U4" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V4" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="Y4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>59</v>
@@ -1382,10 +1511,10 @@
         <v>86</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>89</v>
@@ -1394,49 +1523,67 @@
         <v>90</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N5" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O5" s="5">
         <v>1.0</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="Q5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S5" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U5" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V5" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="Y5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>59</v>
@@ -1448,10 +1595,10 @@
         <v>86</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>89</v>
@@ -1460,49 +1607,67 @@
         <v>90</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N6" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="O6" s="5">
         <v>1.0</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="Q6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U6" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V6" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="Y6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>59</v>
@@ -1514,10 +1679,10 @@
         <v>86</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>89</v>
@@ -1526,49 +1691,67 @@
         <v>90</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N7" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="O7" s="5">
         <v>1.0</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="Q7" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U7" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V7" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="Y7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>59</v>
@@ -1580,10 +1763,10 @@
         <v>86</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>89</v>
@@ -1592,49 +1775,67 @@
         <v>90</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N8" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="O8" s="5">
         <v>1.0</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="Q8" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U8" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V8" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="Y8" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC8" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>59</v>
@@ -1643,13 +1844,13 @@
         <v>60</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>89</v>
@@ -1658,10 +1859,13 @@
         <v>90</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>92</v>
+        <v>139</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="O9" s="5">
         <v>1.0</v>
@@ -1669,36 +1873,51 @@
       <c r="P9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="Q9" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U9" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V9" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X9" s="10"/>
       <c r="Y9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC9" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>59</v>
@@ -1710,10 +1929,10 @@
         <v>86</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>89</v>
@@ -1722,49 +1941,67 @@
         <v>90</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N10" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="O10" s="5">
         <v>1.0</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="Q10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U10" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V10" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X10" s="6" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="Y10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
@@ -1776,10 +2013,10 @@
         <v>86</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>89</v>
@@ -1788,47 +2025,67 @@
         <v>90</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N11" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="O11" s="5">
         <v>1.0</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="Q11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U11" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V11" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W11" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="Y11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="B12" s="5" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>59</v>
@@ -1840,10 +2097,10 @@
         <v>86</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>89</v>
@@ -1852,49 +2109,67 @@
         <v>90</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N12" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="O12" s="5">
         <v>1.0</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="Q12" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S12" s="5" t="s">
         <v>72</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U12" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V12" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="Y12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC12" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z12" s="4"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>59</v>
@@ -1906,10 +2181,10 @@
         <v>86</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>89</v>
@@ -1918,49 +2193,67 @@
         <v>90</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N13" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="O13" s="5">
         <v>1.0</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="Q13" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S13" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U13" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V13" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="Y13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z13" s="4"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>59</v>
@@ -1972,10 +2265,10 @@
         <v>86</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>89</v>
@@ -1984,49 +2277,67 @@
         <v>90</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N14" s="5" t="s">
+        <v>178</v>
+      </c>
       <c r="O14" s="5">
         <v>1.0</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S14" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U14" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V14" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X14" s="6" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="Y14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z14" s="4"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>59</v>
@@ -2038,10 +2349,10 @@
         <v>86</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>89</v>
@@ -2050,49 +2361,67 @@
         <v>90</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N15" s="5" t="s">
+        <v>185</v>
+      </c>
       <c r="O15" s="5">
         <v>1.0</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="Q15" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S15" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U15" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V15" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W15" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X15" s="6" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="Y15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC15" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z15" s="4"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>59</v>
@@ -2104,10 +2433,10 @@
         <v>86</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>89</v>
@@ -2116,49 +2445,67 @@
         <v>90</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N16" s="5" t="s">
+        <v>193</v>
+      </c>
       <c r="O16" s="5">
         <v>1.0</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="Q16" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U16" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V16" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
       <c r="Y16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z16" s="4"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>59</v>
@@ -2170,10 +2517,10 @@
         <v>86</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>89</v>
@@ -2182,49 +2529,67 @@
         <v>90</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N17" s="5" t="s">
+        <v>201</v>
+      </c>
       <c r="O17" s="5">
         <v>1.0</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="Q17" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S17" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U17" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V17" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W17" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X17" s="6" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="Y17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z17" s="4"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>59</v>
@@ -2236,10 +2601,10 @@
         <v>86</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>89</v>
@@ -2248,49 +2613,67 @@
         <v>90</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N18" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="O18" s="5">
         <v>1.0</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="Q18" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S18" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U18" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V18" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X18" s="6" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="Y18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z18" s="4"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>59</v>
@@ -2302,10 +2685,10 @@
         <v>86</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>89</v>
@@ -2314,49 +2697,67 @@
         <v>90</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N19" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="O19" s="5">
         <v>1.0</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="Q19" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S19" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U19" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V19" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X19" s="6" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="Y19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC19" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="Z19" s="4"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>59</v>
@@ -2368,10 +2769,10 @@
         <v>86</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>89</v>
@@ -2380,46 +2781,64 @@
         <v>90</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N20" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="O20" s="5">
         <v>1.0</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="Q20" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S20" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U20" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V20" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="Z20" s="4"/>
+      <c r="AA20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>194</v>
+        <v>228</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>59</v>
@@ -2431,10 +2850,10 @@
         <v>86</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>89</v>
@@ -2443,46 +2862,64 @@
         <v>90</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N21" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="O21" s="5">
         <v>1.0</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="Q21" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S21" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U21" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U21" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V21" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W21" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="Z21" s="4"/>
+      <c r="AA21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>200</v>
+        <v>235</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>59</v>
@@ -2494,10 +2931,10 @@
         <v>86</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>89</v>
@@ -2506,36 +2943,54 @@
         <v>90</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="N22" s="5" t="s">
+        <v>239</v>
+      </c>
       <c r="O22" s="5">
         <v>1.0</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="Q22" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="S22" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U22" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="V22" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W22" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>204</v>
+        <v>241</v>
       </c>
       <c r="Z22" s="4"/>
+      <c r="AA22" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="4"/>

</xml_diff>